<commit_message>
- Main Analysis file
</commit_message>
<xml_diff>
--- a/Association_requiremets.xlsx
+++ b/Association_requiremets.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\TRANSFER_DESKTOP\Homeworks\Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D3B64C-958D-430D-8042-401D1F824D2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9852BAA-677A-423D-8E9E-DCF96931D018}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="758" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="Assoc Rules with traits" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Assoc Rules with traits'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Assoc Rules with traits'!$H$2:$X$23</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Corr variables &amp; traits'!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Metrics of Scott'!$A$1:$C$19</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Rules of Scott'!$A$1:$F$1</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="75">
   <si>
     <t>Variable</t>
   </si>
@@ -242,13 +242,37 @@
   </si>
   <si>
     <t>Correlation Score</t>
+  </si>
+  <si>
+    <t>result in mine</t>
+  </si>
+  <si>
+    <t>Support in mine</t>
+  </si>
+  <si>
+    <t>Confidence in mine</t>
+  </si>
+  <si>
+    <t>Lift in mine</t>
+  </si>
+  <si>
+    <t>Proven</t>
+  </si>
+  <si>
+    <t>Rules of Scott</t>
+  </si>
+  <si>
+    <t>Correlated Variable 1</t>
+  </si>
+  <si>
+    <t>Correlated Variable 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +327,15 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -364,7 +397,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -508,11 +541,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -549,6 +606,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1061,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77853EFD-007B-424F-9043-E2853548FA4D}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection sqref="A1:E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2053,7 +2129,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:D11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2280,618 +2356,1473 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A646984F-8EDA-4CAC-BA3F-A28E3C58EBD7}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C5"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="H1" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
+      <c r="K1" s="42"/>
+      <c r="L1" s="42"/>
+      <c r="M1" s="42"/>
+      <c r="N1" s="42"/>
+      <c r="O1" s="42"/>
+      <c r="P1" s="42"/>
+      <c r="Q1" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" s="42"/>
+      <c r="S1" s="42"/>
+      <c r="T1" s="42"/>
+      <c r="U1" s="42"/>
+      <c r="V1" s="42"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="42"/>
+    </row>
+    <row r="2" spans="1:24" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B2" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C2" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D2" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E2" s="43" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="F2" s="44" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="K2" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="N2" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="O2" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="P2" s="43" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q2" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="T2" s="43" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="V2" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="W2" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="X2" s="43" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D3" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="36" t="str">
+        <f>IF(OR(M3="Yes", U3="Yes"),"Yes", "No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H3" s="34">
+        <v>1</v>
+      </c>
+      <c r="I3" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="K3" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="L3" s="35" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="M3" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="O3" s="45">
+        <v>0.61</v>
+      </c>
+      <c r="P3" s="36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q3" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="S3" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="V3" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="W3" s="45">
+        <v>0.5</v>
+      </c>
+      <c r="X3" s="36">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="34">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B4" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="E4" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F4" s="36" t="str">
+        <f t="shared" ref="F4:F23" si="0">IF(OR(M4="Yes", U4="Yes"),"Yes", "No")</f>
+        <v>Yes</v>
+      </c>
+      <c r="H4" s="34">
+        <v>1</v>
+      </c>
+      <c r="I4" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K4" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="L4" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="O4" s="45">
+        <v>0.08</v>
+      </c>
+      <c r="P4" s="36">
+        <v>0.95</v>
+      </c>
+      <c r="Q4" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="R4" s="35" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="S4" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="U4" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="V4" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="W4" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="X4" s="36">
+        <v>1.17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="37">
+        <v>2</v>
+      </c>
+      <c r="B5" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="D5" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H5" s="37">
+        <v>2</v>
+      </c>
+      <c r="I5" s="38" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="J5" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N5" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="O5" s="45">
+        <v>0.11</v>
+      </c>
+      <c r="P5" s="36">
+        <v>1.28</v>
+      </c>
+      <c r="Q5" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="W5" s="45">
+        <v>0.11</v>
+      </c>
+      <c r="X5" s="36">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="37">
+        <v>2</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H6" s="37">
+        <v>2</v>
+      </c>
+      <c r="I6" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="M6" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="O6" s="45">
+        <v>0.45</v>
+      </c>
+      <c r="P6" s="36">
+        <v>1.28</v>
+      </c>
+      <c r="Q6" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="R6" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="W6" s="45">
+        <v>0.54</v>
+      </c>
+      <c r="X6" s="36">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
+        <v>3</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H7" s="34">
+        <v>3</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="45"/>
+      <c r="N7" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="O7" s="45">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P7" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="Q7" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="R7" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="S7" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="T7" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="W7" s="45">
+        <v>0.15</v>
+      </c>
+      <c r="X7" s="36">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" s="37">
+        <v>4</v>
+      </c>
+      <c r="B8" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H8" s="37">
+        <v>4</v>
+      </c>
+      <c r="I8" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="L8" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="M8" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="O8" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="P8" s="36">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Q8" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="R8" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="S8" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="T8" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45">
+        <v>0.03</v>
+      </c>
+      <c r="W8" s="45">
+        <v>0.1</v>
+      </c>
+      <c r="X8" s="36">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" s="37">
+        <v>4</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H9" s="37">
+        <v>4</v>
+      </c>
+      <c r="I9" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="K9" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="L9" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="M9" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N9" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="O9" s="45">
+        <v>0.47</v>
+      </c>
+      <c r="P9" s="36">
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="Q9" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="T9" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="U9" s="45"/>
+      <c r="V9" s="45">
+        <v>0.03</v>
+      </c>
+      <c r="W9" s="45">
+        <v>0.36</v>
+      </c>
+      <c r="X9" s="36">
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" s="34">
+        <v>5</v>
+      </c>
+      <c r="B10" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H10" s="34">
+        <v>5</v>
+      </c>
+      <c r="I10" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="L10" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="45"/>
+      <c r="N10" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="O10" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="P10" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="Q10" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="R10" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="S10" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="T10" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="W10" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="X10" s="36">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
+        <v>5</v>
+      </c>
+      <c r="B11" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H11" s="34">
+        <v>5</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="K11" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="L11" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="M11" s="45"/>
+      <c r="N11" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="O11" s="45">
+        <v>0.26</v>
+      </c>
+      <c r="P11" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="Q11" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="R11" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="S11" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="T11" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="W11" s="45">
+        <v>0.2</v>
+      </c>
+      <c r="X11" s="36">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" s="37">
+        <v>6</v>
+      </c>
+      <c r="B12" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H12" s="37">
+        <v>6</v>
+      </c>
+      <c r="I12" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="L12" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="M12" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="45">
+        <v>0.11</v>
+      </c>
+      <c r="O12" s="45">
+        <v>0.4</v>
+      </c>
+      <c r="P12" s="36">
+        <v>0.93</v>
+      </c>
+      <c r="Q12" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="R12" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="S12" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="T12" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="U12" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="V12" s="45">
+        <v>0.08</v>
+      </c>
+      <c r="W12" s="45">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X12" s="36">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
+        <v>7</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H13" s="34">
+        <v>7</v>
+      </c>
+      <c r="I13" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="L13" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M13" s="45"/>
+      <c r="N13" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="O13" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="P13" s="36">
+        <v>1.08</v>
+      </c>
+      <c r="Q13" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="R13" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="S13" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="U13" s="45"/>
+      <c r="V13" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="W13" s="45">
+        <v>0.06</v>
+      </c>
+      <c r="X13" s="36">
+        <v>1.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" s="34">
+        <v>7</v>
+      </c>
+      <c r="B14" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H14" s="34">
+        <v>7</v>
+      </c>
+      <c r="I14" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="L14" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="M14" s="45"/>
+      <c r="N14" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="O14" s="45">
+        <v>0.46</v>
+      </c>
+      <c r="P14" s="36">
+        <v>1.08</v>
+      </c>
+      <c r="Q14" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="R14" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="S14" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="T14" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="W14" s="45">
+        <v>0.41</v>
+      </c>
+      <c r="X14" s="36">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A15" s="37">
+        <v>8</v>
+      </c>
+      <c r="B15" s="38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H15" s="37">
+        <v>8</v>
+      </c>
+      <c r="I15" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="J15" s="38" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="L15" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="45"/>
+      <c r="N15" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="O15" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="P15" s="36">
+        <v>0.6</v>
+      </c>
+      <c r="Q15" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="R15" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="S15" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="T15" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45">
+        <v>0.03</v>
+      </c>
+      <c r="W15" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="X15" s="36">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A16" s="34">
+        <v>9</v>
+      </c>
+      <c r="B16" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="F16" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H16" s="34">
+        <v>9</v>
+      </c>
+      <c r="I16" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K16" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="M16" s="45"/>
+      <c r="N16" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="O16" s="45">
+        <v>0.05</v>
+      </c>
+      <c r="P16" s="36">
+        <v>1.45</v>
+      </c>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="36"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="34">
+        <v>9</v>
+      </c>
+      <c r="B17" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H17" s="34">
+        <v>9</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="M17" s="45"/>
+      <c r="N17" s="45">
+        <v>0.02</v>
+      </c>
+      <c r="O17" s="45">
+        <v>0.68</v>
+      </c>
+      <c r="P17" s="36">
+        <v>1.45</v>
+      </c>
+      <c r="Q17" s="47"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="36"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="37">
         <v>10</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="B18" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="38" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>1</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="F18" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H18" s="37">
+        <v>10</v>
+      </c>
+      <c r="I18" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="J18" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="L18" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="M18" s="45"/>
+      <c r="N18" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="O18" s="45">
+        <v>0.08</v>
+      </c>
+      <c r="P18" s="36">
+        <v>0.95</v>
+      </c>
+      <c r="Q18" s="47"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="45"/>
+      <c r="X18" s="36"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A19" s="37">
+        <v>10</v>
+      </c>
+      <c r="B19" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="38" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H19" s="37">
+        <v>10</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="K19" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="M19" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N19" s="45">
+        <v>0.04</v>
+      </c>
+      <c r="O19" s="45">
+        <v>0.44</v>
+      </c>
+      <c r="P19" s="36">
+        <v>0.95</v>
+      </c>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="45"/>
+      <c r="X19" s="36"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="34">
+        <v>11</v>
+      </c>
+      <c r="B20" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H20" s="34">
+        <v>11</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="J20" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="K20" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="L20" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="M20" s="45"/>
+      <c r="N20" s="45">
+        <v>0.01</v>
+      </c>
+      <c r="O20" s="45">
+        <v>0.03</v>
+      </c>
+      <c r="P20" s="36">
+        <v>0.74</v>
+      </c>
+      <c r="Q20" s="47"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="45"/>
+      <c r="W20" s="45"/>
+      <c r="X20" s="36"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="37">
+        <v>12</v>
+      </c>
+      <c r="B21" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="F21" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H21" s="37">
+        <v>12</v>
+      </c>
+      <c r="I21" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="J21" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+      <c r="K21" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="L21" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="M21" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N21" s="45">
+        <v>0.17</v>
+      </c>
+      <c r="O21" s="45">
+        <v>0.31</v>
+      </c>
+      <c r="P21" s="36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="45"/>
+      <c r="W21" s="45"/>
+      <c r="X21" s="36"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="37">
+        <v>12</v>
+      </c>
+      <c r="B22" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="F22" s="36" t="str">
+        <f t="shared" si="0"/>
+        <v>Yes</v>
+      </c>
+      <c r="H22" s="37">
+        <v>12</v>
+      </c>
+      <c r="I22" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" s="38" t="s">
+        <v>4</v>
+      </c>
+      <c r="K22" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="6" t="s">
+      <c r="M22" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="N22" s="45">
+        <v>0.17</v>
+      </c>
+      <c r="O22" s="45">
+        <v>0.6</v>
+      </c>
+      <c r="P22" s="36">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="45"/>
+      <c r="X22" s="36"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="39">
+        <v>13</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="40" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="F23" s="41" t="str">
+        <f t="shared" si="0"/>
+        <v>No</v>
+      </c>
+      <c r="H23" s="39">
+        <v>13</v>
+      </c>
+      <c r="I23" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="J23" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="6" t="s">
+      <c r="K23" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="L23" s="40" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>2</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>2</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>3</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>3</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>4</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>4</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6">
-        <v>4</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6">
-        <v>4</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>5</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>5</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>5</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>5</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="6">
-        <v>6</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
-        <v>6</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>7</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>7</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>7</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
-        <v>7</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
-        <v>8</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
-        <v>8</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>9</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>9</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
-        <v>10</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
-        <v>10</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E31" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>11</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="6">
-        <v>12</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
-        <v>12</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>13</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>8</v>
-      </c>
+      <c r="M23" s="46"/>
+      <c r="N23" s="46">
+        <v>0.03</v>
+      </c>
+      <c r="O23" s="46">
+        <v>0.03</v>
+      </c>
+      <c r="P23" s="41">
+        <v>0.05</v>
+      </c>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="46"/>
+      <c r="S23" s="46"/>
+      <c r="T23" s="46"/>
+      <c r="U23" s="46"/>
+      <c r="V23" s="46"/>
+      <c r="W23" s="46"/>
+      <c r="X23" s="41"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E1" xr:uid="{5595E74D-9D92-4385-AFEF-BDBE7EC577EE}"/>
+  <autoFilter ref="H2:X23" xr:uid="{6BB04A6A-C476-48D5-9463-F0F23A365D6F}"/>
+  <mergeCells count="3">
+    <mergeCell ref="H1:P1"/>
+    <mergeCell ref="Q1:X1"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>